<commit_message>
classification and results pushing added
</commit_message>
<xml_diff>
--- a/tests/testthat/data/df1.xlsx
+++ b/tests/testthat/data/df1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjalocha\Desktop\Mat\Projekty\baseImportance\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjalocha\Desktop\Mat\baseImportance\tests\testthat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57161FA5-4531-49EB-9D1E-DE59E3A46C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F34BF55-0DB1-4D60-85C0-E46762E7C1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9C7A0229-0462-45AA-8ABD-B1E40669C962}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>model_variable</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>MODEL_ID</t>
-  </si>
-  <si>
-    <t>class</t>
   </si>
   <si>
     <t>RF</t>
@@ -437,21 +434,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4219BCE-6D60-40B1-9C78-9A2465732AC2}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,127 +460,103 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>102</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C4">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>102</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C5">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>102</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C7">
+        <v>102</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
-        <v>102</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>102</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C8">
+        <v>102</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>102</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>102</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>